<commit_message>
[server-pipeline] hash_id: commit_msg: ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BF31FE-D05E-425A-97DB-44B8E1FD75CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AttProto" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Admin</author>
   </authors>
   <commentList>
-    <comment ref="P2" authorId="0">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -34,6 +41,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -41,13 +49,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -56,6 +65,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -66,13 +76,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -81,6 +92,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -88,13 +100,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -103,6 +116,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -110,13 +124,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -125,6 +140,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -133,13 +149,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -148,6 +165,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -158,13 +176,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -173,6 +192,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -180,13 +200,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D83" authorId="0">
+    <comment ref="D83" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -195,6 +216,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -335,12 +357,6 @@
     <t>dodge</t>
   </si>
   <si>
-    <t>movescope</t>
-  </si>
-  <si>
-    <t>movetime</t>
-  </si>
-  <si>
     <t>dmgPhysics</t>
   </si>
   <si>
@@ -855,20 +871,24 @@
   </si>
   <si>
     <t>晶石副属性百分比治疗量固定值</t>
+  </si>
+  <si>
+    <t>moveScope</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveTime</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -891,172 +911,36 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="SimSun"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1077,198 +961,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1304,251 +1002,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1593,57 +1049,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1716,6 +1125,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1947,7 +1359,7 @@
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2237,7 +1649,7 @@
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2513,7 +1925,7 @@
           <a:miter lim="400000"/>
         </a:ln>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2786,51 +2198,52 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB96"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.35" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.35" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.625" style="1" customWidth="1"/>
     <col min="5" max="6" width="12.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6166666666667" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" style="1" customWidth="1"/>
     <col min="9" max="10" width="13.875" style="1" customWidth="1"/>
     <col min="11" max="11" width="17.75" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.875" style="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="7.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5416666666667" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" style="1" customWidth="1"/>
     <col min="17" max="17" width="15.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5416666666667" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.15" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.125" style="1" customWidth="1"/>
     <col min="20" max="20" width="12.75" style="1" customWidth="1"/>
     <col min="21" max="21" width="12" style="1" customWidth="1"/>
     <col min="22" max="22" width="16.5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.925" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.875" style="1" customWidth="1"/>
     <col min="24" max="26" width="8" style="1" customWidth="1"/>
     <col min="27" max="28" width="14.5" style="1" customWidth="1"/>
     <col min="29" max="29" width="12.375" style="1" customWidth="1"/>
     <col min="30" max="32" width="14.375" style="1" customWidth="1"/>
     <col min="33" max="52" width="13" style="1" customWidth="1"/>
-    <col min="53" max="54" width="17.35" style="1" customWidth="1"/>
-    <col min="55" max="16384" width="6" style="1" customWidth="1"/>
+    <col min="53" max="54" width="17.375" style="1" customWidth="1"/>
+    <col min="55" max="55" width="6" style="1" customWidth="1"/>
+    <col min="56" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1" spans="1:54">
+    <row r="1" spans="1:54" ht="14.1" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2890,7 +2303,7 @@
       <c r="BA1" s="3"/>
       <c r="BB1" s="3"/>
     </row>
-    <row r="2" ht="113" customHeight="1" spans="1:54">
+    <row r="2" spans="1:54" ht="113.1" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
@@ -3022,7 +2435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="16.15" customHeight="1" spans="1:54">
+    <row r="3" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -3112,244 +2525,244 @@
         <v>39</v>
       </c>
       <c r="AE3" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AK3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AL3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AM3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AP3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AS3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AT3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AU3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AV3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AW3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AX3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AW3" s="8" t="s">
+      <c r="AY3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AX3" s="8" t="s">
+      <c r="AZ3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AY3" s="8" t="s">
+      <c r="BA3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AZ3" s="8" t="s">
+      <c r="BB3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="BA3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="BB3" s="8" t="s">
-        <v>63</v>
-      </c>
     </row>
-    <row r="4" ht="16.15" customHeight="1" spans="1:54">
+    <row r="4" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AC4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AG4" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AH4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AG4" s="8" t="s">
+      <c r="AI4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AH4" s="8" t="s">
+      <c r="AJ4" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AI4" s="8" t="s">
+      <c r="AK4" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AJ4" s="8" t="s">
+      <c r="AL4" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AK4" s="8" t="s">
+      <c r="AM4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AL4" s="8" t="s">
+      <c r="AN4" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AM4" s="8" t="s">
+      <c r="AO4" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AN4" s="8" t="s">
+      <c r="AP4" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AO4" s="8" t="s">
+      <c r="AQ4" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AP4" s="8" t="s">
+      <c r="AR4" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AQ4" s="8" t="s">
+      <c r="AS4" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AR4" s="8" t="s">
+      <c r="AT4" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AS4" s="8" t="s">
+      <c r="AU4" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="AT4" s="8" t="s">
+      <c r="AV4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AU4" s="8" t="s">
+      <c r="AW4" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="AV4" s="8" t="s">
+      <c r="AX4" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AW4" s="8" t="s">
+      <c r="AY4" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AX4" s="8" t="s">
+      <c r="AZ4" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="AY4" s="8" t="s">
+      <c r="BA4" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AZ4" s="8" t="s">
+      <c r="BB4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="BA4" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="BB4" s="8" t="s">
-        <v>115</v>
-      </c>
     </row>
-    <row r="5" ht="16.15" customHeight="1" spans="1:54">
+    <row r="5" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -3404,98 +2817,98 @@
       <c r="BA5" s="8"/>
       <c r="BB5" s="8"/>
     </row>
-    <row r="6" ht="16.15" customHeight="1" spans="1:54">
+    <row r="6" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AB6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AD6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AF6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AG6" s="8"/>
       <c r="AH6" s="8"/>
@@ -3518,20 +2931,20 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="8"/>
       <c r="BA6" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="BB6" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="7" ht="25" customHeight="1" spans="1:54">
+    <row r="7" spans="1:54" ht="24.95" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="9">
         <v>1</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E7" s="11">
         <v>550</v>
@@ -3686,14 +3099,14 @@
         <v>0.15,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="8" ht="25" customHeight="1" spans="1:54">
+    <row r="8" spans="1:54" ht="24.95" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="9">
         <v>2</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" s="11">
         <v>550</v>
@@ -3848,14 +3261,14 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="9" ht="25" customHeight="1" spans="1:54">
+    <row r="9" spans="1:54" ht="24.95" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="9">
         <v>3</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E9" s="11">
         <v>550</v>
@@ -3972,31 +3385,31 @@
         <v>0</v>
       </c>
       <c r="AQ9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AR9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AS9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AT9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AU9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AV9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AW9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AX9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AY9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AZ9" s="12">
         <v>0</v>
@@ -4010,14 +3423,14 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="10" ht="25" customHeight="1" spans="1:54">
+    <row r="10" spans="1:54" ht="24.95" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="9">
         <v>4</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" s="11">
         <v>550</v>
@@ -4110,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="AI10" s="12">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AJ10" s="12">
         <v>0</v>
@@ -4172,14 +3585,14 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="11" ht="16.15" customHeight="1" spans="1:54">
+    <row r="11" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="9">
         <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E11" s="13">
         <v>300</v>
@@ -4334,12 +3747,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="3:54">
+    <row r="12" spans="1:54" ht="13.35" customHeight="1">
       <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" s="13">
         <v>450</v>
@@ -4494,12 +3907,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" customHeight="1" spans="3:54">
+    <row r="13" spans="1:54" ht="13.35" customHeight="1">
       <c r="C13" s="1">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" s="13">
         <v>550</v>
@@ -4654,12 +4067,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="14" customHeight="1" spans="3:54">
+    <row r="14" spans="1:54" ht="13.35" customHeight="1">
       <c r="C14" s="1">
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E14" s="1">
         <v>75</v>
@@ -4814,12 +4227,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="3:54">
+    <row r="15" spans="1:54" ht="13.35" customHeight="1">
       <c r="C15" s="1">
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E15" s="1">
         <v>125</v>
@@ -4974,12 +4387,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="3:54">
+    <row r="16" spans="1:54" ht="13.35" customHeight="1">
       <c r="C16" s="1">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E16" s="1">
         <v>175</v>
@@ -5134,12 +4547,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="3:54">
+    <row r="17" spans="2:54" ht="13.35" customHeight="1">
       <c r="C17" s="1">
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E17" s="1">
         <v>225</v>
@@ -5294,12 +4707,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="3:54">
+    <row r="18" spans="2:54" ht="13.35" customHeight="1">
       <c r="C18" s="1">
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E18" s="1">
         <v>275</v>
@@ -5454,12 +4867,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="3:54">
+    <row r="19" spans="2:54" ht="13.35" customHeight="1">
       <c r="C19" s="1">
         <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E19" s="1">
         <v>10</v>
@@ -5614,12 +5027,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="3:54">
+    <row r="20" spans="2:54" ht="13.35" customHeight="1">
       <c r="C20" s="1">
         <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E20" s="13">
         <v>50</v>
@@ -5774,12 +5187,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="21" customHeight="1" spans="3:54">
+    <row r="21" spans="2:54" ht="13.35" customHeight="1">
       <c r="C21" s="1">
         <v>2000</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E21" s="1">
         <v>50</v>
@@ -5934,12 +5347,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="22" customHeight="1" spans="3:54">
+    <row r="22" spans="2:54" ht="13.35" customHeight="1">
       <c r="C22" s="1">
         <v>2001</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E22" s="1">
         <v>10</v>
@@ -6094,15 +5507,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="2:54">
+    <row r="23" spans="2:54" ht="13.35" customHeight="1">
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C23" s="1">
         <v>2010</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -6114,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="12">
-        <v>0.047</v>
+        <v>4.7E-2</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -6257,15 +5670,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="24" customHeight="1" spans="2:54">
+    <row r="24" spans="2:54" ht="13.35" customHeight="1">
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="1">
         <v>2011</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -6277,7 +5690,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="12">
-        <v>0.072</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -6420,15 +5833,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="2:54">
+    <row r="25" spans="2:54" ht="13.35" customHeight="1">
       <c r="B25" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C25" s="1">
         <v>2012</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -6440,7 +5853,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="12">
-        <v>0.097</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -6583,15 +5996,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="26" customHeight="1" spans="2:54">
+    <row r="26" spans="2:54" ht="13.35" customHeight="1">
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" s="1">
         <v>2013</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -6746,15 +6159,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="27" customHeight="1" spans="2:54">
+    <row r="27" spans="2:54" ht="13.35" customHeight="1">
       <c r="B27" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C27" s="1">
         <v>2014</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -6766,7 +6179,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="12">
-        <v>0.147</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -6909,15 +6322,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="2:54">
+    <row r="28" spans="2:54" ht="13.35" customHeight="1">
       <c r="B28" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1">
         <v>2020</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -7072,15 +6485,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="2:54">
+    <row r="29" spans="2:54" ht="13.35" customHeight="1">
       <c r="B29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C29" s="1">
         <v>2021</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -7235,15 +6648,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="2:54">
+    <row r="30" spans="2:54" ht="13.35" customHeight="1">
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C30" s="1">
         <v>2022</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -7398,15 +6811,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="2:54">
+    <row r="31" spans="2:54" ht="13.35" customHeight="1">
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1">
         <v>2023</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -7561,15 +6974,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="32" customHeight="1" spans="2:54">
+    <row r="32" spans="2:54" ht="13.35" customHeight="1">
       <c r="B32" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C32" s="1">
         <v>2024</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -7724,12 +7137,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="33" customHeight="1" spans="3:54">
+    <row r="33" spans="3:54" ht="13.35" customHeight="1">
       <c r="C33" s="1">
         <v>3000</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E33" s="1">
         <v>6</v>
@@ -7884,12 +7297,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="34" customHeight="1" spans="3:54">
+    <row r="34" spans="3:54" ht="13.35" customHeight="1">
       <c r="C34" s="1">
         <v>3001</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E34" s="1">
         <v>60</v>
@@ -8044,12 +7457,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="35" customHeight="1" spans="3:54">
+    <row r="35" spans="3:54" ht="13.35" customHeight="1">
       <c r="C35" s="1">
         <v>3010</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E35" s="1">
         <v>120</v>
@@ -8204,12 +7617,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="36" customHeight="1" spans="3:54">
+    <row r="36" spans="3:54" ht="13.35" customHeight="1">
       <c r="C36" s="1">
         <v>3011</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E36" s="1">
         <v>1200</v>
@@ -8364,12 +7777,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="37" customHeight="1" spans="3:54">
+    <row r="37" spans="3:54" ht="13.35" customHeight="1">
       <c r="C37" s="1">
         <v>3020</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E37" s="1">
         <v>6</v>
@@ -8524,12 +7937,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="38" customHeight="1" spans="3:54">
+    <row r="38" spans="3:54" ht="13.35" customHeight="1">
       <c r="C38" s="1">
         <v>3021</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E38" s="1">
         <v>60</v>
@@ -8684,12 +8097,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="3:54">
+    <row r="39" spans="3:54" ht="13.35" customHeight="1">
       <c r="C39" s="1">
         <v>3030</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -8734,7 +8147,7 @@
         <v>0</v>
       </c>
       <c r="S39" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="T39" s="1">
         <v>0</v>
@@ -8844,12 +8257,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="40" customHeight="1" spans="3:54">
+    <row r="40" spans="3:54" ht="13.35" customHeight="1">
       <c r="C40" s="1">
         <v>3031</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -8894,7 +8307,7 @@
         <v>0</v>
       </c>
       <c r="S40" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="T40" s="1">
         <v>0</v>
@@ -9004,12 +8417,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="41" customHeight="1" spans="3:54">
+    <row r="41" spans="3:54" ht="13.35" customHeight="1">
       <c r="C41" s="1">
         <v>3032</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -9048,7 +8461,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="R41" s="1">
         <v>0</v>
@@ -9164,12 +8577,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="42" customHeight="1" spans="3:54">
+    <row r="42" spans="3:54" ht="13.35" customHeight="1">
       <c r="C42" s="1">
         <v>3033</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -9208,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="R42" s="1">
         <v>0</v>
@@ -9324,12 +8737,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="43" customHeight="1" spans="3:54">
+    <row r="43" spans="3:54" ht="13.35" customHeight="1">
       <c r="C43" s="1">
         <v>3034</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -9359,7 +8772,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="12">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="O43" s="1">
         <v>0</v>
@@ -9484,12 +8897,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="44" customHeight="1" spans="3:54">
+    <row r="44" spans="3:54" ht="13.35" customHeight="1">
       <c r="C44" s="1">
         <v>3035</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -9519,7 +8932,7 @@
         <v>0</v>
       </c>
       <c r="N44" s="12">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O44" s="1">
         <v>0</v>
@@ -9644,12 +9057,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="45" customHeight="1" spans="3:54">
+    <row r="45" spans="3:54" ht="13.35" customHeight="1">
       <c r="C45" s="1">
         <v>3036</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -9804,12 +9217,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="46" customHeight="1" spans="3:54">
+    <row r="46" spans="3:54" ht="13.35" customHeight="1">
       <c r="C46" s="1">
         <v>3037</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -9964,12 +9377,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="47" customHeight="1" spans="3:54">
+    <row r="47" spans="3:54" ht="13.35" customHeight="1">
       <c r="C47" s="1">
         <v>3050</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -10059,7 +9472,7 @@
         <v>0</v>
       </c>
       <c r="AH47" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AI47" s="1">
         <v>0</v>
@@ -10124,12 +9537,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="48" customHeight="1" spans="3:54">
+    <row r="48" spans="3:54" ht="13.35" customHeight="1">
       <c r="C48" s="1">
         <v>3051</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -10222,7 +9635,7 @@
         <v>0</v>
       </c>
       <c r="AI48" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AJ48" s="1">
         <v>0</v>
@@ -10284,12 +9697,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="49" customHeight="1" spans="3:54">
+    <row r="49" spans="3:54" ht="13.35" customHeight="1">
       <c r="C49" s="1">
         <v>3052</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -10385,7 +9798,7 @@
         <v>0</v>
       </c>
       <c r="AJ49" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AK49" s="1">
         <v>0</v>
@@ -10444,12 +9857,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="50" customHeight="1" spans="3:54">
+    <row r="50" spans="3:54" ht="13.35" customHeight="1">
       <c r="C50" s="1">
         <v>3053</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -10548,7 +9961,7 @@
         <v>0</v>
       </c>
       <c r="AK50" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AL50" s="1">
         <v>0</v>
@@ -10604,12 +10017,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="51" customHeight="1" spans="3:54">
+    <row r="51" spans="3:54" ht="13.35" customHeight="1">
       <c r="C51" s="1">
         <v>3054</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -10711,7 +10124,7 @@
         <v>0</v>
       </c>
       <c r="AL51" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AM51" s="1">
         <v>0</v>
@@ -10764,12 +10177,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="52" customHeight="1" spans="3:54">
+    <row r="52" spans="3:54" ht="13.35" customHeight="1">
       <c r="C52" s="1">
         <v>3055</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -10874,7 +10287,7 @@
         <v>0</v>
       </c>
       <c r="AM52" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AN52" s="1">
         <v>0</v>
@@ -10924,12 +10337,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="53" customHeight="1" spans="3:54">
+    <row r="53" spans="3:54" ht="13.35" customHeight="1">
       <c r="C53" s="1">
         <v>3056</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -11037,7 +10450,7 @@
         <v>0</v>
       </c>
       <c r="AN53" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AO53" s="1">
         <v>0</v>
@@ -11076,20 +10489,20 @@
         <v>0</v>
       </c>
       <c r="BA53" s="10" t="str">
-        <f t="shared" ref="BA48:BA82" si="6">AG47:AG57&amp;","&amp;AH47:AH57&amp;","&amp;AI47:AI57&amp;","&amp;AJ47:AJ57&amp;","&amp;AK47:AK57&amp;","&amp;AL47:AL57&amp;","&amp;AM47:AM57&amp;","&amp;AN47:AN57&amp;","&amp;AO47:AO57&amp;","&amp;AP47:AP57</f>
+        <f t="shared" ref="BA53:BA82" si="6">AG47:AG57&amp;","&amp;AH47:AH57&amp;","&amp;AI47:AI57&amp;","&amp;AJ47:AJ57&amp;","&amp;AK47:AK57&amp;","&amp;AL47:AL57&amp;","&amp;AM47:AM57&amp;","&amp;AN47:AN57&amp;","&amp;AO47:AO57&amp;","&amp;AP47:AP57</f>
         <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
       <c r="BB53" s="10" t="str">
-        <f t="shared" ref="BB48:BB82" si="7">AQ47:AQ57&amp;","&amp;AR47:AR57&amp;","&amp;AS47:AS57&amp;","&amp;AT47:AT57&amp;","&amp;AU47:AU57&amp;","&amp;AV47:AV57&amp;","&amp;AW47:AW57&amp;","&amp;AX47:AX57&amp;","&amp;AY47:AY57&amp;","&amp;AZ47:AZ57</f>
+        <f t="shared" ref="BB53:BB82" si="7">AQ47:AQ57&amp;","&amp;AR47:AR57&amp;","&amp;AS47:AS57&amp;","&amp;AT47:AT57&amp;","&amp;AU47:AU57&amp;","&amp;AV47:AV57&amp;","&amp;AW47:AW57&amp;","&amp;AX47:AX57&amp;","&amp;AY47:AY57&amp;","&amp;AZ47:AZ57</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="54" customHeight="1" spans="3:54">
+    <row r="54" spans="3:54" ht="13.35" customHeight="1">
       <c r="C54" s="1">
         <v>3057</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -11200,7 +10613,7 @@
         <v>0</v>
       </c>
       <c r="AO54" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AP54" s="1">
         <v>0</v>
@@ -11244,12 +10657,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="55" customHeight="1" spans="3:54">
+    <row r="55" spans="3:54" ht="13.35" customHeight="1">
       <c r="C55" s="1">
         <v>3058</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -11363,7 +10776,7 @@
         <v>0</v>
       </c>
       <c r="AP55" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AQ55" s="1">
         <v>0</v>
@@ -11404,12 +10817,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="56" customHeight="1" spans="3:54">
+    <row r="56" spans="3:54" ht="13.35" customHeight="1">
       <c r="C56" s="1">
         <v>3059</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -11499,7 +10912,7 @@
         <v>0</v>
       </c>
       <c r="AH56" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AI56" s="1">
         <v>0</v>
@@ -11564,12 +10977,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="57" customHeight="1" spans="3:54">
+    <row r="57" spans="3:54" ht="13.35" customHeight="1">
       <c r="C57" s="1">
         <v>3060</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -11662,7 +11075,7 @@
         <v>0</v>
       </c>
       <c r="AI57" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AJ57" s="1">
         <v>0</v>
@@ -11724,12 +11137,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="58" customHeight="1" spans="3:54">
+    <row r="58" spans="3:54" ht="13.35" customHeight="1">
       <c r="C58" s="1">
         <v>3061</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -11825,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="AJ58" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AK58" s="1">
         <v>0</v>
@@ -11884,12 +11297,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="59" customHeight="1" spans="3:54">
+    <row r="59" spans="3:54" ht="13.35" customHeight="1">
       <c r="C59" s="1">
         <v>3062</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -11988,7 +11401,7 @@
         <v>0</v>
       </c>
       <c r="AK59" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AL59" s="1">
         <v>0</v>
@@ -12044,12 +11457,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="60" customHeight="1" spans="3:54">
+    <row r="60" spans="3:54" ht="13.35" customHeight="1">
       <c r="C60" s="1">
         <v>3063</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -12151,7 +11564,7 @@
         <v>0</v>
       </c>
       <c r="AL60" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AM60" s="1">
         <v>0</v>
@@ -12204,12 +11617,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="61" customHeight="1" spans="3:54">
+    <row r="61" spans="3:54" ht="13.35" customHeight="1">
       <c r="C61" s="1">
         <v>3064</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
@@ -12314,7 +11727,7 @@
         <v>0</v>
       </c>
       <c r="AM61" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AN61" s="1">
         <v>0</v>
@@ -12364,12 +11777,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="62" customHeight="1" spans="3:54">
+    <row r="62" spans="3:54" ht="13.35" customHeight="1">
       <c r="C62" s="1">
         <v>3065</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E62" s="1">
         <v>0</v>
@@ -12477,7 +11890,7 @@
         <v>0</v>
       </c>
       <c r="AN62" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AO62" s="1">
         <v>0</v>
@@ -12524,12 +11937,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="63" customHeight="1" spans="3:54">
+    <row r="63" spans="3:54" ht="13.35" customHeight="1">
       <c r="C63" s="1">
         <v>3066</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E63" s="1">
         <v>0</v>
@@ -12640,7 +12053,7 @@
         <v>0</v>
       </c>
       <c r="AO63" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AP63" s="1">
         <v>0</v>
@@ -12684,12 +12097,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="64" customHeight="1" spans="3:54">
+    <row r="64" spans="3:54" ht="13.35" customHeight="1">
       <c r="C64" s="1">
         <v>3067</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E64" s="1">
         <v>0</v>
@@ -12803,7 +12216,7 @@
         <v>0</v>
       </c>
       <c r="AP64" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ64" s="1">
         <v>0</v>
@@ -12844,12 +12257,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="65" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="65" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C65" s="2">
         <v>3068</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E65" s="2">
         <v>0</v>
@@ -12969,7 +12382,7 @@
         <v>0</v>
       </c>
       <c r="AR65" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS65" s="2">
         <v>0</v>
@@ -13004,12 +12417,12 @@
         <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="66" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="66" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C66" s="2">
         <v>3069</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E66" s="2">
         <v>0</v>
@@ -13132,7 +12545,7 @@
         <v>0</v>
       </c>
       <c r="AS66" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AT66" s="2">
         <v>0</v>
@@ -13164,12 +12577,12 @@
         <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="67" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="67" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C67" s="2">
         <v>3070</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E67" s="2">
         <v>0</v>
@@ -13295,7 +12708,7 @@
         <v>0</v>
       </c>
       <c r="AT67" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AU67" s="2">
         <v>0</v>
@@ -13324,12 +12737,12 @@
         <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="68" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="68" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C68" s="2">
         <v>3071</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E68" s="2">
         <v>0</v>
@@ -13458,7 +12871,7 @@
         <v>0</v>
       </c>
       <c r="AU68" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AV68" s="2">
         <v>0</v>
@@ -13484,12 +12897,12 @@
         <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="69" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="69" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C69" s="2">
         <v>3072</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -13621,7 +13034,7 @@
         <v>0</v>
       </c>
       <c r="AV69" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AW69" s="2">
         <v>0</v>
@@ -13644,12 +13057,12 @@
         <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
     </row>
-    <row r="70" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="70" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C70" s="2">
         <v>3073</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
@@ -13784,7 +13197,7 @@
         <v>0</v>
       </c>
       <c r="AW70" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AX70" s="2">
         <v>0</v>
@@ -13804,12 +13217,12 @@
         <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
     </row>
-    <row r="71" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="71" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C71" s="2">
         <v>3074</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E71" s="2">
         <v>0</v>
@@ -13947,7 +13360,7 @@
         <v>0</v>
       </c>
       <c r="AX71" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AY71" s="2">
         <v>0</v>
@@ -13964,12 +13377,12 @@
         <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
     </row>
-    <row r="72" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="72" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C72" s="2">
         <v>3075</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E72" s="2">
         <v>0</v>
@@ -14110,7 +13523,7 @@
         <v>0</v>
       </c>
       <c r="AY72" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AZ72" s="2">
         <v>0</v>
@@ -14124,12 +13537,12 @@
         <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
     </row>
-    <row r="73" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="73" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C73" s="2">
         <v>3076</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E73" s="2">
         <v>0</v>
@@ -14284,12 +13697,12 @@
         <v>0,0,0,0,0,0,0,0,0,20</v>
       </c>
     </row>
-    <row r="74" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="74" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C74" s="2">
         <v>3077</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E74" s="2">
         <v>0</v>
@@ -14409,7 +13822,7 @@
         <v>0</v>
       </c>
       <c r="AR74" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AS74" s="2">
         <v>0</v>
@@ -14444,12 +13857,12 @@
         <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="75" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="75" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C75" s="2">
         <v>3078</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -14572,7 +13985,7 @@
         <v>0</v>
       </c>
       <c r="AS75" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT75" s="2">
         <v>0</v>
@@ -14604,12 +14017,12 @@
         <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="76" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="76" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C76" s="2">
         <v>3079</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -14735,7 +14148,7 @@
         <v>0</v>
       </c>
       <c r="AT76" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AU76" s="2">
         <v>0</v>
@@ -14764,12 +14177,12 @@
         <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="77" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="77" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C77" s="2">
         <v>3080</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -14898,7 +14311,7 @@
         <v>0</v>
       </c>
       <c r="AU77" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AV77" s="2">
         <v>0</v>
@@ -14924,12 +14337,12 @@
         <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="78" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="78" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C78" s="2">
         <v>3081</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -15061,7 +14474,7 @@
         <v>0</v>
       </c>
       <c r="AV78" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AW78" s="2">
         <v>0</v>
@@ -15084,12 +14497,12 @@
         <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
     </row>
-    <row r="79" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="79" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C79" s="2">
         <v>3082</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -15224,7 +14637,7 @@
         <v>0</v>
       </c>
       <c r="AW79" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AX79" s="2">
         <v>0</v>
@@ -15244,12 +14657,12 @@
         <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
     </row>
-    <row r="80" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="80" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C80" s="2">
         <v>3083</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E80" s="2">
         <v>0</v>
@@ -15387,7 +14800,7 @@
         <v>0</v>
       </c>
       <c r="AX80" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AY80" s="2">
         <v>0</v>
@@ -15404,12 +14817,12 @@
         <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
     </row>
-    <row r="81" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="81" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C81" s="2">
         <v>3084</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E81" s="2">
         <v>0</v>
@@ -15550,7 +14963,7 @@
         <v>0</v>
       </c>
       <c r="AY81" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AZ81" s="2">
         <v>0</v>
@@ -15564,12 +14977,12 @@
         <v>0,0,0,0,0,0,0,0,0.005,0</v>
       </c>
     </row>
-    <row r="82" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="82" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C82" s="2">
         <v>3085</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
@@ -15724,12 +15137,12 @@
         <v>0,0,0,0,0,0,0,0,0,50</v>
       </c>
     </row>
-    <row r="83" customHeight="1" spans="3:54">
+    <row r="83" spans="3:54" ht="13.35" customHeight="1">
       <c r="C83" s="1">
         <v>3200</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E83" s="1">
         <v>36</v>
@@ -15884,12 +15297,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="84" customHeight="1" spans="3:54">
+    <row r="84" spans="3:54" ht="13.35" customHeight="1">
       <c r="C84" s="1">
         <v>3201</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E84" s="1">
         <v>0</v>
@@ -16044,12 +15457,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="85" customHeight="1" spans="3:54">
+    <row r="85" spans="3:54" ht="13.35" customHeight="1">
       <c r="C85" s="1">
         <v>3202</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E85" s="1">
         <v>0</v>
@@ -16204,18 +15617,18 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="86" customHeight="1" spans="3:54">
+    <row r="86" spans="3:54" ht="13.35" customHeight="1">
       <c r="C86" s="1">
         <v>3203</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E86" s="1">
         <v>0</v>
       </c>
       <c r="F86" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="G86" s="1">
         <v>0</v>
@@ -16364,12 +15777,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="87" customHeight="1" spans="3:54">
+    <row r="87" spans="3:54" ht="13.35" customHeight="1">
       <c r="C87" s="1">
         <v>3204</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E87" s="1">
         <v>0</v>
@@ -16381,7 +15794,7 @@
         <v>0</v>
       </c>
       <c r="H87" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I87" s="1">
         <v>0</v>
@@ -16524,12 +15937,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="88" customHeight="1" spans="3:54">
+    <row r="88" spans="3:54" ht="13.35" customHeight="1">
       <c r="C88" s="1">
         <v>3205</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E88" s="1">
         <v>0</v>
@@ -16586,7 +15999,7 @@
         <v>0</v>
       </c>
       <c r="W88" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="X88" s="1">
         <v>0</v>
@@ -16684,12 +16097,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="89" customHeight="1" spans="3:54">
+    <row r="89" spans="3:54" ht="13.35" customHeight="1">
       <c r="C89" s="1">
         <v>3206</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E89" s="1">
         <v>0</v>
@@ -16844,12 +16257,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="90" customHeight="1" spans="3:54">
+    <row r="90" spans="3:54" ht="13.35" customHeight="1">
       <c r="C90" s="1">
         <v>3207</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E90" s="1">
         <v>0</v>
@@ -17004,12 +16417,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="91" customHeight="1" spans="3:54">
+    <row r="91" spans="3:54" ht="13.35" customHeight="1">
       <c r="C91" s="1">
         <v>3208</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E91" s="1">
         <v>0</v>
@@ -17164,12 +16577,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="92" customHeight="1" spans="3:54">
+    <row r="92" spans="3:54" ht="13.35" customHeight="1">
       <c r="C92" s="1">
         <v>3209</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E92" s="1">
         <v>0</v>
@@ -17324,12 +16737,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="93" customHeight="1" spans="3:54">
+    <row r="93" spans="3:54" ht="13.35" customHeight="1">
       <c r="C93" s="1">
         <v>3210</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E93" s="1">
         <v>0</v>
@@ -17484,12 +16897,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="94" customHeight="1" spans="3:54">
+    <row r="94" spans="3:54" ht="13.35" customHeight="1">
       <c r="C94" s="1">
         <v>3211</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E94" s="1">
         <v>0</v>
@@ -17534,7 +16947,7 @@
         <v>0</v>
       </c>
       <c r="S94" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="T94" s="1">
         <v>0</v>
@@ -17644,12 +17057,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="95" customHeight="1" spans="3:54">
+    <row r="95" spans="3:54" ht="13.35" customHeight="1">
       <c r="C95" s="1">
         <v>3212</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E95" s="1">
         <v>0</v>
@@ -17688,7 +17101,7 @@
         <v>0</v>
       </c>
       <c r="Q95" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="R95" s="1">
         <v>0</v>
@@ -17804,12 +17217,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="96" customHeight="1" spans="3:54">
+    <row r="96" spans="3:54" ht="13.35" customHeight="1">
       <c r="C96" s="1">
         <v>3213</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E96" s="1">
         <v>0</v>
@@ -17839,7 +17252,7 @@
         <v>0</v>
       </c>
       <c r="N96" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="O96" s="1">
         <v>0</v>
@@ -17965,11 +17378,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>